<commit_message>
Ajuste documentação Tela Principal
</commit_message>
<xml_diff>
--- a/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
+++ b/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Epicos!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Story!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Tasks!$A$1:$E$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Tasks!$A$1:$E$105</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Temas!$A$1:$D$1</definedName>
     <definedName name="CodEpico">Epicos!$C$2:$C$10</definedName>
     <definedName name="CodTema">Temas!$B$2:$B$10</definedName>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="129">
   <si>
     <t>Tema</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Acesso aos Módulos</t>
   </si>
   <si>
-    <t>Acessar a tela principal</t>
-  </si>
-  <si>
     <t>T1 - EP1 - EU1</t>
   </si>
   <si>
@@ -412,6 +409,18 @@
   </si>
   <si>
     <t>Excluir Filmes – Opção Sim</t>
+  </si>
+  <si>
+    <t>Tela principal – Acesso</t>
+  </si>
+  <si>
+    <t>Tela principal – Abre a tela de gêneros</t>
+  </si>
+  <si>
+    <t>Tela principal – Abre a tela de Idiomas</t>
+  </si>
+  <si>
+    <t>Tela principal – Abre a tela de Filmes</t>
   </si>
 </sst>
 </file>
@@ -671,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -747,11 +756,26 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="46">
     <dxf>
       <border>
         <left style="thin">
@@ -1111,6 +1135,215 @@
         </top>
         <bottom style="thin">
           <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -2019,7 +2252,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2503,7 +2736,7 @@
       </c>
       <c r="E2" s="21">
         <f t="shared" ref="E2:E7" si="3">COUNTIF(StatusTasks,A2)</f>
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2673,7 +2906,7 @@
         <v>T2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>6</v>
@@ -2688,7 +2921,7 @@
         <v>T3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>6</v>
@@ -4068,27 +4301,27 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A1:C100 B3:B200">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="10">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="35" priority="2" operator="containsText" text="Pronto">
+    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="Pronto">
       <formula>NOT(ISERROR(SEARCH("Pronto",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="3" operator="containsText" text="Em Testes">
+    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="Em Testes">
       <formula>NOT(ISERROR(SEARCH("Em Testes",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="Completo">
+    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="Completo">
       <formula>NOT(ISERROR(SEARCH("Completo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="Em Desenvolvimento">
+    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="Em Desenvolvimento">
       <formula>NOT(ISERROR(SEARCH("Em Desenvolvimento",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="6" operator="containsText" text="Aceito">
+    <cfRule type="containsText" dxfId="40" priority="6" operator="containsText" text="Aceito">
       <formula>NOT(ISERROR(SEARCH("Aceito",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="Aguardando">
+    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="Aguardando">
       <formula>NOT(ISERROR(SEARCH("Aguardando",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4158,7 +4391,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
@@ -4168,7 +4401,7 @@
         <v>T2 - EP1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>6</v>
@@ -4176,7 +4409,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7">
         <v>2</v>
@@ -4186,7 +4419,7 @@
         <v>T2 - EP2</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>6</v>
@@ -4194,7 +4427,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
@@ -4204,7 +4437,7 @@
         <v>T3 - EP1</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>6</v>
@@ -5662,27 +5895,27 @@
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <conditionalFormatting sqref="A1:D100 C3:C199">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="10">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="Pronto">
+    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="Pronto">
       <formula>NOT(ISERROR(SEARCH("Pronto",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="Em Testes">
+    <cfRule type="containsText" dxfId="36" priority="3" operator="containsText" text="Em Testes">
       <formula>NOT(ISERROR(SEARCH("Em Testes",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="Completo">
+    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="Completo">
       <formula>NOT(ISERROR(SEARCH("Completo",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="Em Desenvolvimento">
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="Em Desenvolvimento">
       <formula>NOT(ISERROR(SEARCH("Em Desenvolvimento",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="Aceito">
+    <cfRule type="containsText" dxfId="33" priority="6" operator="containsText" text="Aceito">
       <formula>NOT(ISERROR(SEARCH("Aceito",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="Aguardando">
+    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="Aguardando">
       <formula>NOT(ISERROR(SEARCH("Aguardando",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5758,7 +5991,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
@@ -5768,7 +6001,7 @@
         <v>T2 - EP1 - EU1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>6</v>
@@ -5776,7 +6009,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="7">
         <v>2</v>
@@ -5786,7 +6019,7 @@
         <v>T2 - EP1 - EU2</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>6</v>
@@ -5794,7 +6027,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="7">
         <v>3</v>
@@ -5804,7 +6037,7 @@
         <v>T2 - EP1 - EU3</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>6</v>
@@ -5812,7 +6045,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="7">
         <v>4</v>
@@ -5822,7 +6055,7 @@
         <v>T2 - EP1 - EU4</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>6</v>
@@ -5830,7 +6063,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
@@ -5840,7 +6073,7 @@
         <v>T2 - EP2 - EU1</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>6</v>
@@ -5848,7 +6081,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="7">
         <v>2</v>
@@ -5858,7 +6091,7 @@
         <v>T2 - EP2 - EU2</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>6</v>
@@ -5866,7 +6099,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="7">
         <v>3</v>
@@ -5876,7 +6109,7 @@
         <v>T2 - EP2 - EU3</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>6</v>
@@ -5884,7 +6117,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="7">
         <v>4</v>
@@ -5894,7 +6127,7 @@
         <v>T2 - EP2 - EU4</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>6</v>
@@ -5902,7 +6135,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="7">
         <v>1</v>
@@ -5912,7 +6145,7 @@
         <v>T3 - EP1 - EU1</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>6</v>
@@ -5920,7 +6153,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="7">
         <v>2</v>
@@ -5930,7 +6163,7 @@
         <v>T3 - EP1 - EU2</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>6</v>
@@ -5938,7 +6171,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="7">
         <v>3</v>
@@ -5948,7 +6181,7 @@
         <v>T3 - EP1 - EU3</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>6</v>
@@ -5956,7 +6189,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="7">
         <v>4</v>
@@ -5966,7 +6199,7 @@
         <v>T3 - EP1 - EU4</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>6</v>
@@ -7349,27 +7582,27 @@
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <conditionalFormatting sqref="C3:C200 A1:D100">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="15">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Pronto">
+    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="Pronto">
       <formula>NOT(ISERROR(SEARCH("Pronto",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="Em Testes">
+    <cfRule type="containsText" dxfId="29" priority="3" operator="containsText" text="Em Testes">
       <formula>NOT(ISERROR(SEARCH("Em Testes",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="Completo">
+    <cfRule type="containsText" dxfId="28" priority="4" operator="containsText" text="Completo">
       <formula>NOT(ISERROR(SEARCH("Completo",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="5" operator="containsText" text="Em Desenvolvimento">
+    <cfRule type="containsText" dxfId="27" priority="5" operator="containsText" text="Em Desenvolvimento">
       <formula>NOT(ISERROR(SEARCH("Em Desenvolvimento",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="6" operator="containsText" text="Aceito">
+    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="Aceito">
       <formula>NOT(ISERROR(SEARCH("Aceito",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="Aguardando">
+    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="Aguardando">
       <formula>NOT(ISERROR(SEARCH("Aguardando",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7388,31 +7621,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="41" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="41" customWidth="1"/>
+    <col min="4" max="4" width="73" style="3" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="9" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="38" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="38" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="15" t="s">
@@ -7423,2147 +7656,2201 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="32" t="s">
-        <v>24</v>
+      <c r="A2" s="39" t="s">
+        <v>23</v>
       </c>
       <c r="B2" s="32">
         <v>1</v>
       </c>
-      <c r="C2" s="32" t="str">
+      <c r="C2" s="39" t="str">
         <f>IF(A2&lt;&gt;"",A2&amp;" - C"&amp;B2,"")</f>
         <v>T1 - EP1 - EU1 - C1</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="29">
+      <c r="A3" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="32">
+        <v>2</v>
+      </c>
+      <c r="C3" s="39" t="str">
+        <f>IF(A3&lt;&gt;"",A3&amp;" - C"&amp;B3,"")</f>
+        <v>T1 - EP1 - EU1 - C2</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="32">
+        <v>3</v>
+      </c>
+      <c r="C4" s="39" t="str">
+        <f t="shared" ref="C4:C5" si="0">IF(A4&lt;&gt;"",A4&amp;" - C"&amp;B4,"")</f>
+        <v>T1 - EP1 - EU1 - C3</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="32">
+        <v>4</v>
+      </c>
+      <c r="C5" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>T1 - EP1 - EU1 - C4</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="29">
         <v>1</v>
       </c>
-      <c r="C3" s="29" t="str">
-        <f>IF(A3&lt;&gt;"",A3&amp;" - C"&amp;B3,"")</f>
+      <c r="C6" s="37" t="str">
+        <f>IF(A6&lt;&gt;"",A6&amp;" - C"&amp;B6,"")</f>
         <v>T2 - EP1 - EU1 - C1</v>
       </c>
-      <c r="D3" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="29">
-        <v>2</v>
-      </c>
-      <c r="C4" s="29" t="str">
-        <f t="shared" ref="C4:C68" si="0">IF(A4&lt;&gt;"",A4&amp;" - C"&amp;B4,"")</f>
-        <v>T2 - EP1 - EU1 - C2</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="29">
-        <v>3</v>
-      </c>
-      <c r="C5" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU1 - C3</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="29">
-        <v>4</v>
-      </c>
-      <c r="C6" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU1 - C4</v>
-      </c>
       <c r="D6" s="30" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="29">
+        <v>2</v>
+      </c>
+      <c r="C7" s="37" t="str">
+        <f t="shared" ref="C7:C71" si="1">IF(A7&lt;&gt;"",A7&amp;" - C"&amp;B7,"")</f>
+        <v>T2 - EP1 - EU1 - C2</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="29">
+        <v>3</v>
+      </c>
+      <c r="C8" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU1 - C3</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="29">
+        <v>4</v>
+      </c>
+      <c r="C9" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU1 - C4</v>
+      </c>
+      <c r="D9" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="32">
+      <c r="E9" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="32">
         <v>1</v>
       </c>
-      <c r="C7" s="32" t="str">
-        <f t="shared" si="0"/>
+      <c r="C10" s="39" t="str">
+        <f t="shared" si="1"/>
         <v>T2 - EP1 - EU2 - C1</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="32">
-        <v>2</v>
-      </c>
-      <c r="C8" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU2 - C2</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="32">
-        <v>3</v>
-      </c>
-      <c r="C9" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU2 - C3</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="32">
-        <v>4</v>
-      </c>
-      <c r="C10" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU2 - C4</v>
-      </c>
       <c r="D10" s="33" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="29">
+      <c r="A11" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="32">
+        <v>2</v>
+      </c>
+      <c r="C11" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU2 - C2</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="32">
+        <v>3</v>
+      </c>
+      <c r="C12" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU2 - C3</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="32">
+        <v>4</v>
+      </c>
+      <c r="C13" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU2 - C4</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="29">
         <v>1</v>
       </c>
-      <c r="C11" s="29" t="str">
-        <f t="shared" si="0"/>
+      <c r="C14" s="37" t="str">
+        <f t="shared" si="1"/>
         <v>T2 - EP1 - EU3 - C1</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="29">
-        <v>2</v>
-      </c>
-      <c r="C12" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU3 - C2</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="29">
-        <v>3</v>
-      </c>
-      <c r="C13" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU3 - C3</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="29">
-        <v>4</v>
-      </c>
-      <c r="C14" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU3 - C4</v>
-      </c>
       <c r="D14" s="30" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="29">
+        <v>2</v>
+      </c>
+      <c r="C15" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU3 - C2</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="29">
+        <v>3</v>
+      </c>
+      <c r="C16" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU3 - C3</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="29">
+        <v>4</v>
+      </c>
+      <c r="C17" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU3 - C4</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="32">
         <v>1</v>
       </c>
-      <c r="C15" s="32" t="str">
-        <f t="shared" si="0"/>
+      <c r="C18" s="39" t="str">
+        <f t="shared" si="1"/>
         <v>T2 - EP1 - EU4 - C1</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D18" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="32">
+        <v>2</v>
+      </c>
+      <c r="C19" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU4 - C2</v>
+      </c>
+      <c r="D19" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E19" s="34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="32">
-        <v>2</v>
-      </c>
-      <c r="C16" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU4 - C2</v>
-      </c>
-      <c r="D16" s="33" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="32">
+        <v>3</v>
+      </c>
+      <c r="C20" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP1 - EU4 - C3</v>
+      </c>
+      <c r="D20" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E20" s="34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="32">
-        <v>3</v>
-      </c>
-      <c r="C17" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP1 - EU4 - C3</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="29">
+    <row r="21" spans="1:5">
+      <c r="A21" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="29">
         <v>1</v>
       </c>
-      <c r="C18" s="29" t="str">
-        <f t="shared" si="0"/>
+      <c r="C21" s="37" t="str">
+        <f t="shared" si="1"/>
         <v>T2 - EP2 - EU1 - C1</v>
       </c>
-      <c r="D18" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="29">
-        <v>2</v>
-      </c>
-      <c r="C19" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU1 - C2</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="29">
-        <v>3</v>
-      </c>
-      <c r="C20" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU1 - C3</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="29">
-        <v>4</v>
-      </c>
-      <c r="C21" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU1 - C4</v>
-      </c>
       <c r="D21" s="35" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="29">
+        <v>2</v>
+      </c>
+      <c r="C22" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU1 - C2</v>
+      </c>
+      <c r="D22" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="32">
+      <c r="E22" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="29">
+        <v>3</v>
+      </c>
+      <c r="C23" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU1 - C3</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="29">
+        <v>4</v>
+      </c>
+      <c r="C24" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU1 - C4</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="32">
         <v>1</v>
       </c>
-      <c r="C22" s="32" t="str">
-        <f t="shared" si="0"/>
+      <c r="C25" s="39" t="str">
+        <f t="shared" si="1"/>
         <v>T2 - EP2 - EU2 - C1</v>
       </c>
-      <c r="D22" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="32">
-        <v>2</v>
-      </c>
-      <c r="C23" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU2 - C2</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="32">
-        <v>3</v>
-      </c>
-      <c r="C24" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU2 - C3</v>
-      </c>
-      <c r="D24" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="32">
-        <v>4</v>
-      </c>
-      <c r="C25" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU2 - C4</v>
-      </c>
       <c r="D25" s="36" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E25" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="29">
+      <c r="A26" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="32">
+        <v>2</v>
+      </c>
+      <c r="C26" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU2 - C2</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="32">
+        <v>3</v>
+      </c>
+      <c r="C27" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU2 - C3</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="32">
+        <v>4</v>
+      </c>
+      <c r="C28" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU2 - C4</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="29">
         <v>1</v>
       </c>
-      <c r="C26" s="29" t="str">
-        <f t="shared" si="0"/>
+      <c r="C29" s="37" t="str">
+        <f t="shared" si="1"/>
         <v>T2 - EP2 - EU3 - C1</v>
       </c>
-      <c r="D26" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="29">
-        <v>2</v>
-      </c>
-      <c r="C27" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU3 - C2</v>
-      </c>
-      <c r="D27" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="29">
-        <v>3</v>
-      </c>
-      <c r="C28" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU3 - C3</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="29">
-        <v>4</v>
-      </c>
-      <c r="C29" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU3 - C4</v>
-      </c>
       <c r="D29" s="35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E29" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="32">
+      <c r="A30" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="29">
+        <v>2</v>
+      </c>
+      <c r="C30" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU3 - C2</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="29">
+        <v>3</v>
+      </c>
+      <c r="C31" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU3 - C3</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="29">
+        <v>4</v>
+      </c>
+      <c r="C32" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU3 - C4</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="32">
         <v>1</v>
       </c>
-      <c r="C30" s="32" t="str">
-        <f t="shared" si="0"/>
+      <c r="C33" s="39" t="str">
+        <f t="shared" si="1"/>
         <v>T2 - EP2 - EU4 - C1</v>
       </c>
-      <c r="D30" s="36" t="s">
+      <c r="D33" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="32">
+        <v>2</v>
+      </c>
+      <c r="C34" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU4 - C2</v>
+      </c>
+      <c r="D34" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E34" s="34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="32">
-        <v>2</v>
-      </c>
-      <c r="C31" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU4 - C2</v>
-      </c>
-      <c r="D31" s="36" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="32">
+        <v>3</v>
+      </c>
+      <c r="C35" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T2 - EP2 - EU4 - C3</v>
+      </c>
+      <c r="D35" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E35" s="34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="32">
-        <v>3</v>
-      </c>
-      <c r="C32" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T2 - EP2 - EU4 - C3</v>
-      </c>
-      <c r="D32" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="29" t="s">
+    <row r="36" spans="1:5">
+      <c r="A36" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="29">
+        <v>1</v>
+      </c>
+      <c r="C36" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU1 - C1</v>
+      </c>
+      <c r="D36" s="35" t="s">
         <v>83</v>
-      </c>
-      <c r="B33" s="29">
-        <v>1</v>
-      </c>
-      <c r="C33" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU1 - C1</v>
-      </c>
-      <c r="D33" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" s="29">
-        <v>2</v>
-      </c>
-      <c r="C34" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU1 - C2</v>
-      </c>
-      <c r="D34" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" s="29">
-        <v>3</v>
-      </c>
-      <c r="C35" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU1 - C3</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="29">
-        <v>4</v>
-      </c>
-      <c r="C36" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU1 - C4</v>
-      </c>
-      <c r="D36" s="35" t="s">
-        <v>87</v>
       </c>
       <c r="E36" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="29" t="s">
-        <v>83</v>
+      <c r="A37" s="37" t="s">
+        <v>82</v>
       </c>
       <c r="B37" s="29">
-        <v>5</v>
-      </c>
-      <c r="C37" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU1 - C5</v>
+        <v>2</v>
+      </c>
+      <c r="C37" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU1 - C2</v>
       </c>
       <c r="D37" s="35" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E37" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="29" t="s">
-        <v>83</v>
+      <c r="A38" s="37" t="s">
+        <v>82</v>
       </c>
       <c r="B38" s="29">
-        <v>6</v>
-      </c>
-      <c r="C38" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU1 - C6</v>
+        <v>3</v>
+      </c>
+      <c r="C38" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU1 - C3</v>
       </c>
       <c r="D38" s="35" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E38" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="29" t="s">
-        <v>83</v>
+      <c r="A39" s="37" t="s">
+        <v>82</v>
       </c>
       <c r="B39" s="29">
-        <v>7</v>
-      </c>
-      <c r="C39" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU1 - C7</v>
+        <v>4</v>
+      </c>
+      <c r="C39" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU1 - C4</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E39" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="29" t="s">
-        <v>83</v>
+      <c r="A40" s="37" t="s">
+        <v>82</v>
       </c>
       <c r="B40" s="29">
-        <v>8</v>
-      </c>
-      <c r="C40" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU1 - C8</v>
+        <v>5</v>
+      </c>
+      <c r="C40" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU1 - C5</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E40" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="29">
+        <v>6</v>
+      </c>
+      <c r="C41" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU1 - C6</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="29">
+        <v>7</v>
+      </c>
+      <c r="C42" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU1 - C7</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="29">
+        <v>8</v>
+      </c>
+      <c r="C43" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU1 - C8</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="32">
+        <v>1</v>
+      </c>
+      <c r="C44" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C1</v>
+      </c>
+      <c r="D44" s="36" t="s">
         <v>92</v>
-      </c>
-      <c r="B41" s="32">
-        <v>1</v>
-      </c>
-      <c r="C41" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C1</v>
-      </c>
-      <c r="D41" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="E41" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42" s="32">
-        <v>2</v>
-      </c>
-      <c r="C42" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C2</v>
-      </c>
-      <c r="D42" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="32">
-        <v>3</v>
-      </c>
-      <c r="C43" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C3</v>
-      </c>
-      <c r="D43" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="E43" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="32">
-        <v>4</v>
-      </c>
-      <c r="C44" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C4</v>
-      </c>
-      <c r="D44" s="36" t="s">
-        <v>96</v>
       </c>
       <c r="E44" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="32" t="s">
-        <v>92</v>
+      <c r="A45" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B45" s="32">
-        <v>5</v>
-      </c>
-      <c r="C45" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C5</v>
+        <v>2</v>
+      </c>
+      <c r="C45" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C2</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E45" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="32" t="s">
-        <v>92</v>
+      <c r="A46" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B46" s="32">
-        <v>6</v>
-      </c>
-      <c r="C46" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C6</v>
+        <v>3</v>
+      </c>
+      <c r="C46" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C3</v>
       </c>
       <c r="D46" s="36" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E46" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="32" t="s">
-        <v>92</v>
+      <c r="A47" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B47" s="32">
-        <v>7</v>
-      </c>
-      <c r="C47" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C7</v>
+        <v>4</v>
+      </c>
+      <c r="C47" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C4</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E47" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="32" t="s">
-        <v>92</v>
+      <c r="A48" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B48" s="32">
-        <v>8</v>
-      </c>
-      <c r="C48" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C8</v>
+        <v>5</v>
+      </c>
+      <c r="C48" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C5</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E48" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="32" t="s">
-        <v>92</v>
+      <c r="A49" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B49" s="32">
-        <v>9</v>
-      </c>
-      <c r="C49" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C9</v>
+        <v>6</v>
+      </c>
+      <c r="C49" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C6</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E49" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="32" t="s">
-        <v>92</v>
+      <c r="A50" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B50" s="32">
-        <v>10</v>
-      </c>
-      <c r="C50" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C10</v>
+        <v>7</v>
+      </c>
+      <c r="C50" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C7</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E50" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="32" t="s">
-        <v>92</v>
+      <c r="A51" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B51" s="32">
-        <v>11</v>
-      </c>
-      <c r="C51" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C11</v>
+        <v>8</v>
+      </c>
+      <c r="C51" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C8</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E51" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="32" t="s">
-        <v>92</v>
+      <c r="A52" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B52" s="32">
-        <v>12</v>
-      </c>
-      <c r="C52" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C12</v>
+        <v>9</v>
+      </c>
+      <c r="C52" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C9</v>
       </c>
       <c r="D52" s="36" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E52" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="32" t="s">
-        <v>92</v>
+      <c r="A53" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B53" s="32">
-        <v>13</v>
-      </c>
-      <c r="C53" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C13</v>
+        <v>10</v>
+      </c>
+      <c r="C53" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C10</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E53" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="32" t="s">
-        <v>92</v>
+      <c r="A54" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B54" s="32">
-        <v>14</v>
-      </c>
-      <c r="C54" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU2 - C14</v>
+        <v>11</v>
+      </c>
+      <c r="C54" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C11</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E54" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" s="29">
+      <c r="A55" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="32">
+        <v>12</v>
+      </c>
+      <c r="C55" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C12</v>
+      </c>
+      <c r="D55" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="E55" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="32">
+        <v>13</v>
+      </c>
+      <c r="C56" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C13</v>
+      </c>
+      <c r="D56" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="32">
+        <v>14</v>
+      </c>
+      <c r="C57" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU2 - C14</v>
+      </c>
+      <c r="D57" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="29">
         <v>1</v>
       </c>
-      <c r="C55" s="29" t="str">
-        <f t="shared" si="0"/>
+      <c r="C58" s="37" t="str">
+        <f t="shared" si="1"/>
         <v>T3 - EP1 - EU3 - C1</v>
       </c>
-      <c r="D55" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="E55" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="B56" s="29">
-        <v>2</v>
-      </c>
-      <c r="C56" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C2</v>
-      </c>
-      <c r="D56" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="B57" s="29">
-        <v>3</v>
-      </c>
-      <c r="C57" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C3</v>
-      </c>
-      <c r="D57" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="E57" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="B58" s="29">
-        <v>4</v>
-      </c>
-      <c r="C58" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C4</v>
-      </c>
       <c r="D58" s="35" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E58" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="29" t="s">
-        <v>107</v>
+      <c r="A59" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B59" s="29">
-        <v>5</v>
-      </c>
-      <c r="C59" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C5</v>
+        <v>2</v>
+      </c>
+      <c r="C59" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C2</v>
       </c>
       <c r="D59" s="35" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E59" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="29" t="s">
-        <v>107</v>
+      <c r="A60" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B60" s="29">
-        <v>6</v>
-      </c>
-      <c r="C60" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C6</v>
+        <v>3</v>
+      </c>
+      <c r="C60" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C3</v>
       </c>
       <c r="D60" s="35" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E60" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="29" t="s">
-        <v>107</v>
+      <c r="A61" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B61" s="29">
-        <v>7</v>
-      </c>
-      <c r="C61" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C7</v>
+        <v>4</v>
+      </c>
+      <c r="C61" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C4</v>
       </c>
       <c r="D61" s="35" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E61" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="29" t="s">
-        <v>107</v>
+      <c r="A62" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B62" s="29">
-        <v>8</v>
-      </c>
-      <c r="C62" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C8</v>
+        <v>5</v>
+      </c>
+      <c r="C62" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C5</v>
       </c>
       <c r="D62" s="35" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E62" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="29" t="s">
-        <v>107</v>
+      <c r="A63" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B63" s="29">
-        <v>9</v>
-      </c>
-      <c r="C63" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C9</v>
+        <v>6</v>
+      </c>
+      <c r="C63" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C6</v>
       </c>
       <c r="D63" s="35" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E63" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="29" t="s">
-        <v>107</v>
+      <c r="A64" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B64" s="29">
-        <v>10</v>
-      </c>
-      <c r="C64" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C10</v>
+        <v>7</v>
+      </c>
+      <c r="C64" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C7</v>
       </c>
       <c r="D64" s="35" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E64" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="29" t="s">
-        <v>107</v>
+      <c r="A65" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B65" s="29">
-        <v>11</v>
-      </c>
-      <c r="C65" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C11</v>
+        <v>8</v>
+      </c>
+      <c r="C65" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C8</v>
       </c>
       <c r="D65" s="35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E65" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="29" t="s">
-        <v>107</v>
+      <c r="A66" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B66" s="29">
-        <v>12</v>
-      </c>
-      <c r="C66" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C12</v>
+        <v>9</v>
+      </c>
+      <c r="C66" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C9</v>
       </c>
       <c r="D66" s="35" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E66" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="29" t="s">
-        <v>107</v>
+      <c r="A67" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B67" s="29">
-        <v>13</v>
-      </c>
-      <c r="C67" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C13</v>
+        <v>10</v>
+      </c>
+      <c r="C67" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C10</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E67" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="29" t="s">
-        <v>107</v>
+      <c r="A68" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B68" s="29">
-        <v>14</v>
-      </c>
-      <c r="C68" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>T3 - EP1 - EU3 - C14</v>
+        <v>11</v>
+      </c>
+      <c r="C68" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C11</v>
       </c>
       <c r="D68" s="35" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E68" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="29" t="s">
-        <v>107</v>
+      <c r="A69" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="B69" s="29">
-        <v>15</v>
-      </c>
-      <c r="C69" s="29" t="str">
-        <f t="shared" ref="C69:C132" si="1">IF(A69&lt;&gt;"",A69&amp;" - C"&amp;B69,"")</f>
-        <v>T3 - EP1 - EU3 - C15</v>
+        <v>12</v>
+      </c>
+      <c r="C69" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C12</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E69" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B70" s="32">
+      <c r="A70" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="29">
+        <v>13</v>
+      </c>
+      <c r="C70" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C13</v>
+      </c>
+      <c r="D70" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="E70" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="29">
+        <v>14</v>
+      </c>
+      <c r="C71" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>T3 - EP1 - EU3 - C14</v>
+      </c>
+      <c r="D71" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="E71" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="29">
+        <v>15</v>
+      </c>
+      <c r="C72" s="37" t="str">
+        <f t="shared" ref="C72:C135" si="2">IF(A72&lt;&gt;"",A72&amp;" - C"&amp;B72,"")</f>
+        <v>T3 - EP1 - EU3 - C15</v>
+      </c>
+      <c r="D72" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="E72" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B73" s="32">
         <v>1</v>
       </c>
-      <c r="C70" s="32" t="str">
-        <f t="shared" si="1"/>
+      <c r="C73" s="39" t="str">
+        <f t="shared" si="2"/>
         <v>T3 - EP1 - EU4 - C1</v>
       </c>
-      <c r="D70" s="36" t="s">
+      <c r="D73" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="E73" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B74" s="32">
+        <v>2</v>
+      </c>
+      <c r="C74" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v>T3 - EP1 - EU4 - C2</v>
+      </c>
+      <c r="D74" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="E70" s="34" t="s">
+      <c r="E74" s="34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B71" s="32">
-        <v>2</v>
-      </c>
-      <c r="C71" s="32" t="str">
-        <f t="shared" si="1"/>
-        <v>T3 - EP1 - EU4 - C2</v>
-      </c>
-      <c r="D71" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E71" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D72" s="8"/>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D73" s="8"/>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D74" s="8"/>
-    </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="7"/>
+      <c r="A75" s="40"/>
       <c r="B75" s="7"/>
-      <c r="C75" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C75" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D75" s="8"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="7"/>
+      <c r="A76" s="40"/>
       <c r="B76" s="7"/>
-      <c r="C76" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C76" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D76" s="8"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="7"/>
+      <c r="A77" s="40"/>
       <c r="B77" s="7"/>
-      <c r="C77" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C77" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="7"/>
+      <c r="A78" s="40"/>
       <c r="B78" s="7"/>
-      <c r="C78" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C78" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="7"/>
+      <c r="A79" s="40"/>
       <c r="B79" s="7"/>
-      <c r="C79" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C79" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="7"/>
+      <c r="A80" s="40"/>
       <c r="B80" s="7"/>
-      <c r="C80" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C80" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="7"/>
+      <c r="A81" s="40"/>
       <c r="B81" s="7"/>
-      <c r="C81" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C81" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D81" s="8"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="7"/>
+      <c r="A82" s="40"/>
       <c r="B82" s="7"/>
-      <c r="C82" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C82" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D82" s="8"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="7"/>
+      <c r="A83" s="40"/>
       <c r="B83" s="7"/>
-      <c r="C83" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C83" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D83" s="8"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="7"/>
+      <c r="A84" s="40"/>
       <c r="B84" s="7"/>
-      <c r="C84" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C84" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D84" s="8"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="7"/>
+      <c r="A85" s="40"/>
       <c r="B85" s="7"/>
-      <c r="C85" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C85" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D85" s="8"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="7"/>
+      <c r="A86" s="40"/>
       <c r="B86" s="7"/>
-      <c r="C86" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C86" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D86" s="8"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="7"/>
+      <c r="A87" s="40"/>
       <c r="B87" s="7"/>
-      <c r="C87" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C87" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D87" s="8"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="7"/>
+      <c r="A88" s="40"/>
       <c r="B88" s="7"/>
-      <c r="C88" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C88" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D88" s="8"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="7"/>
+      <c r="A89" s="40"/>
       <c r="B89" s="7"/>
-      <c r="C89" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C89" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D89" s="8"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="7"/>
+      <c r="A90" s="40"/>
       <c r="B90" s="7"/>
-      <c r="C90" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C90" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D90" s="8"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="7"/>
+      <c r="A91" s="40"/>
       <c r="B91" s="7"/>
-      <c r="C91" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C91" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D91" s="8"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="7"/>
+      <c r="A92" s="40"/>
       <c r="B92" s="7"/>
-      <c r="C92" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C92" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D92" s="8"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="7"/>
+      <c r="A93" s="40"/>
       <c r="B93" s="7"/>
-      <c r="C93" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C93" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D93" s="8"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="7"/>
+      <c r="A94" s="40"/>
       <c r="B94" s="7"/>
-      <c r="C94" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C94" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D94" s="8"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="7"/>
+      <c r="A95" s="40"/>
       <c r="B95" s="7"/>
-      <c r="C95" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C95" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D95" s="8"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="7"/>
+      <c r="A96" s="40"/>
       <c r="B96" s="7"/>
-      <c r="C96" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C96" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D96" s="8"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="7"/>
+      <c r="A97" s="40"/>
       <c r="B97" s="7"/>
-      <c r="C97" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C97" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D97" s="8"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="7"/>
+      <c r="A98" s="40"/>
       <c r="B98" s="7"/>
-      <c r="C98" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C98" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D98" s="8"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="7"/>
+      <c r="A99" s="40"/>
       <c r="B99" s="7"/>
-      <c r="C99" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C99" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D99" s="8"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="7"/>
+      <c r="A100" s="40"/>
       <c r="B100" s="7"/>
-      <c r="C100" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C100" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D100" s="8"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="7"/>
+      <c r="A101" s="40"/>
       <c r="B101" s="7"/>
-      <c r="C101" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C101" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D101" s="8"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="7"/>
+      <c r="A102" s="40"/>
       <c r="B102" s="7"/>
-      <c r="C102" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C102" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D102" s="8"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="C103" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A103" s="40"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D103" s="8"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="C104" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A104" s="40"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D104" s="8"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="C105" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A105" s="40"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D105" s="8"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="C106" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C106" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:4">
-      <c r="C107" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C107" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="1:4">
-      <c r="C108" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C108" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="1:4">
-      <c r="C109" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C109" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="1:4">
-      <c r="C110" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C110" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="1:4">
-      <c r="C111" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C111" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="1:4">
-      <c r="C112" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C112" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="3:3">
-      <c r="C113" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C113" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="3:3">
-      <c r="C114" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C114" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="3:3">
-      <c r="C115" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C115" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="3:3">
-      <c r="C116" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C116" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="3:3">
-      <c r="C117" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C117" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="3:3">
-      <c r="C118" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C118" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="3:3">
-      <c r="C119" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C119" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="3:3">
-      <c r="C120" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C120" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="3:3">
-      <c r="C121" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C121" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="3:3">
-      <c r="C122" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C122" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="3:3">
-      <c r="C123" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C123" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="3:3">
-      <c r="C124" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C124" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="3:3">
-      <c r="C125" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C125" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="3:3">
-      <c r="C126" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C126" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="3:3">
-      <c r="C127" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C127" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="3:3">
-      <c r="C128" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C128" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="3:3">
-      <c r="C129" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C129" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="3:3">
-      <c r="C130" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C130" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="131" spans="3:3">
-      <c r="C131" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C131" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="132" spans="3:3">
-      <c r="C132" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="C132" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="133" spans="3:3">
-      <c r="C133" s="7" t="str">
-        <f t="shared" ref="C133:C196" si="2">IF(A133&lt;&gt;"",A133&amp;" - C"&amp;B133,"")</f>
+      <c r="C133" s="40" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="3:3">
-      <c r="C134" s="7" t="str">
+      <c r="C134" s="40" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="3:3">
-      <c r="C135" s="7" t="str">
+      <c r="C135" s="40" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="3:3">
-      <c r="C136" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C136" s="40" t="str">
+        <f t="shared" ref="C136:C199" si="3">IF(A136&lt;&gt;"",A136&amp;" - C"&amp;B136,"")</f>
         <v/>
       </c>
     </row>
     <row r="137" spans="3:3">
-      <c r="C137" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C137" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="138" spans="3:3">
-      <c r="C138" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C138" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="139" spans="3:3">
-      <c r="C139" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C139" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="140" spans="3:3">
-      <c r="C140" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C140" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="141" spans="3:3">
-      <c r="C141" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C141" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="3:3">
-      <c r="C142" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C142" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="3:3">
-      <c r="C143" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C143" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="3:3">
-      <c r="C144" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C144" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="3:3">
-      <c r="C145" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C145" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="146" spans="3:3">
-      <c r="C146" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C146" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="147" spans="3:3">
-      <c r="C147" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C147" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="148" spans="3:3">
-      <c r="C148" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C148" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="149" spans="3:3">
-      <c r="C149" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C149" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="150" spans="3:3">
-      <c r="C150" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C150" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="3:3">
-      <c r="C151" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C151" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="152" spans="3:3">
-      <c r="C152" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C152" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="153" spans="3:3">
-      <c r="C153" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C153" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="154" spans="3:3">
-      <c r="C154" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C154" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="155" spans="3:3">
-      <c r="C155" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C155" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="156" spans="3:3">
-      <c r="C156" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C156" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="157" spans="3:3">
-      <c r="C157" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C157" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="158" spans="3:3">
-      <c r="C158" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C158" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="159" spans="3:3">
-      <c r="C159" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C159" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="160" spans="3:3">
-      <c r="C160" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C160" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="161" spans="3:3">
-      <c r="C161" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C161" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="162" spans="3:3">
-      <c r="C162" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C162" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="163" spans="3:3">
-      <c r="C163" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C163" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="164" spans="3:3">
-      <c r="C164" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C164" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="165" spans="3:3">
-      <c r="C165" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C165" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="166" spans="3:3">
-      <c r="C166" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C166" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="167" spans="3:3">
-      <c r="C167" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C167" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="168" spans="3:3">
-      <c r="C168" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C168" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="169" spans="3:3">
-      <c r="C169" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C169" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="170" spans="3:3">
-      <c r="C170" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C170" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="171" spans="3:3">
-      <c r="C171" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C171" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="172" spans="3:3">
-      <c r="C172" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C172" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="173" spans="3:3">
-      <c r="C173" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C173" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="174" spans="3:3">
-      <c r="C174" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C174" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="175" spans="3:3">
-      <c r="C175" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C175" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="176" spans="3:3">
-      <c r="C176" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C176" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="177" spans="3:3">
-      <c r="C177" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C177" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="178" spans="3:3">
-      <c r="C178" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C178" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="179" spans="3:3">
-      <c r="C179" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C179" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="180" spans="3:3">
-      <c r="C180" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C180" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="181" spans="3:3">
-      <c r="C181" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C181" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="182" spans="3:3">
-      <c r="C182" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C182" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="183" spans="3:3">
-      <c r="C183" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C183" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="184" spans="3:3">
-      <c r="C184" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C184" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="185" spans="3:3">
-      <c r="C185" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C185" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="186" spans="3:3">
-      <c r="C186" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C186" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="187" spans="3:3">
-      <c r="C187" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C187" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="188" spans="3:3">
-      <c r="C188" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C188" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="189" spans="3:3">
-      <c r="C189" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C189" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="190" spans="3:3">
-      <c r="C190" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C190" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="191" spans="3:3">
-      <c r="C191" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C191" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="192" spans="3:3">
-      <c r="C192" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C192" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="193" spans="3:3">
-      <c r="C193" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C193" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="194" spans="3:3">
-      <c r="C194" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C194" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="195" spans="3:3">
-      <c r="C195" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C195" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="196" spans="3:3">
-      <c r="C196" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="C196" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="197" spans="3:3">
-      <c r="C197" s="7" t="str">
-        <f t="shared" ref="C197:C202" si="3">IF(A197&lt;&gt;"",A197&amp;" - C"&amp;B197,"")</f>
+      <c r="C197" s="40" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="198" spans="3:3">
-      <c r="C198" s="7" t="str">
+      <c r="C198" s="40" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="199" spans="3:3">
-      <c r="C199" s="7" t="str">
+      <c r="C199" s="40" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="200" spans="3:3">
-      <c r="C200" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="C200" s="40" t="str">
+        <f t="shared" ref="C200:C205" si="4">IF(A200&lt;&gt;"",A200&amp;" - C"&amp;B200,"")</f>
         <v/>
       </c>
     </row>
     <row r="201" spans="3:3">
-      <c r="C201" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="C201" s="40" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="202" spans="3:3">
-      <c r="C202" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="C202" s="40" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="203" spans="3:3">
+      <c r="C203" s="40" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="204" spans="3:3">
+      <c r="C204" s="40" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="205" spans="3:3">
+      <c r="C205" s="40" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E102"/>
-  <conditionalFormatting sqref="C3:C202 D3:D4 D6:D102 A2:C102">
+  <autoFilter ref="A1:E105"/>
+  <conditionalFormatting sqref="C6:C205 D9:D105 A2:C105 D2:D7">
     <cfRule type="notContainsBlanks" dxfId="1" priority="8">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
@@ -9589,10 +9876,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A105">
       <formula1>CodUserStory</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E105">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Criação da tela principal
</commit_message>
<xml_diff>
--- a/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
+++ b/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Graficos" sheetId="7" r:id="rId1"/>
@@ -775,43 +775,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <b/>
@@ -944,388 +908,6 @@
         </top>
         <bottom style="thin">
           <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1916,7 +1498,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2108,10 +1689,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2127,25 +1708,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133831680"/>
-        <c:axId val="133853952"/>
+        <c:axId val="107899904"/>
+        <c:axId val="107918080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133831680"/>
+        <c:axId val="107899904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133853952"/>
+        <c:crossAx val="107918080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133853952"/>
+        <c:axId val="107918080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2167,25 +1748,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133831680"/>
+        <c:crossAx val="107899904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000113" footer="0.31496062000000113"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000125" footer="0.31496062000000125"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2195,9 +1774,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -2274,24 +1851,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133870720"/>
-        <c:axId val="133872256"/>
+        <c:axId val="107930752"/>
+        <c:axId val="107932288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133870720"/>
+        <c:axId val="107930752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133872256"/>
+        <c:crossAx val="107932288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133872256"/>
+        <c:axId val="107932288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2299,20 +1876,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133870720"/>
+        <c:crossAx val="107930752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000047" footer="0.31496062000000047"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2753,7 +2329,7 @@
       </c>
       <c r="D3" s="23">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="24">
         <f t="shared" si="3"/>
@@ -2774,7 +2350,7 @@
       </c>
       <c r="D4" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="24">
         <f t="shared" si="3"/>
@@ -4301,27 +3877,27 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A1:C100 B3:B200">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="10">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="Pronto">
+    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="Pronto">
       <formula>NOT(ISERROR(SEARCH("Pronto",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="Em Testes">
+    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="Em Testes">
       <formula>NOT(ISERROR(SEARCH("Em Testes",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="Completo">
+    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Completo">
       <formula>NOT(ISERROR(SEARCH("Completo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="Em Desenvolvimento">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Em Desenvolvimento">
       <formula>NOT(ISERROR(SEARCH("Em Desenvolvimento",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="6" operator="containsText" text="Aceito">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Aceito">
       <formula>NOT(ISERROR(SEARCH("Aceito",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="Aguardando">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Aguardando">
       <formula>NOT(ISERROR(SEARCH("Aguardando",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5895,27 +5471,27 @@
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <conditionalFormatting sqref="A1:D100 C3:C199">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="10">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="Pronto">
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="Pronto">
       <formula>NOT(ISERROR(SEARCH("Pronto",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="3" operator="containsText" text="Em Testes">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Em Testes">
       <formula>NOT(ISERROR(SEARCH("Em Testes",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="Completo">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Completo">
       <formula>NOT(ISERROR(SEARCH("Completo",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="Em Desenvolvimento">
+    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="Em Desenvolvimento">
       <formula>NOT(ISERROR(SEARCH("Em Desenvolvimento",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="6" operator="containsText" text="Aceito">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Aceito">
       <formula>NOT(ISERROR(SEARCH("Aceito",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="Aguardando">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="Aguardando">
       <formula>NOT(ISERROR(SEARCH("Aguardando",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5939,9 +5515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -5986,7 +5562,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -7582,27 +7158,27 @@
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <conditionalFormatting sqref="C3:C200 A1:D100">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="Pronto">
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="Pronto">
       <formula>NOT(ISERROR(SEARCH("Pronto",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="3" operator="containsText" text="Em Testes">
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Em Testes">
       <formula>NOT(ISERROR(SEARCH("Em Testes",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="4" operator="containsText" text="Completo">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Completo">
       <formula>NOT(ISERROR(SEARCH("Completo",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="5" operator="containsText" text="Em Desenvolvimento">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Em Desenvolvimento">
       <formula>NOT(ISERROR(SEARCH("Em Desenvolvimento",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="Aceito">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Aceito">
       <formula>NOT(ISERROR(SEARCH("Aceito",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="Aguardando">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Aguardando">
       <formula>NOT(ISERROR(SEARCH("Aguardando",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7623,9 +7199,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -9851,27 +9427,27 @@
   </sheetData>
   <autoFilter ref="A1:E105"/>
   <conditionalFormatting sqref="C6:C205 D9:D105 A2:C105 D2:D7">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Aguardando">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Aguardando">
       <formula>NOT(ISERROR(SEARCH("Aguardando",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Pronto">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Pronto">
       <formula>NOT(ISERROR(SEARCH("Pronto",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Em Testes">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Em Testes">
       <formula>NOT(ISERROR(SEARCH("Em Testes",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Completo">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Completo">
       <formula>NOT(ISERROR(SEARCH("Completo",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Em Desenvolvimento">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Em Desenvolvimento">
       <formula>NOT(ISERROR(SEARCH("Em Desenvolvimento",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Aceito">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Aceito">
       <formula>NOT(ISERROR(SEARCH("Aceito",E1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ajuste Documentação tela inicial
</commit_message>
<xml_diff>
--- a/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
+++ b/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Graficos" sheetId="7" r:id="rId1"/>
@@ -1498,6 +1498,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1553,10 +1554,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1621,10 +1622,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1748,6 +1749,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1759,6 +1761,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1774,7 +1777,9 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1883,6 +1888,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2321,11 +2327,11 @@
       </c>
       <c r="B3" s="23">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C3" s="23">
+        <f t="shared" si="1"/>
         <v>3</v>
-      </c>
-      <c r="C3" s="23">
-        <f t="shared" si="1"/>
-        <v>4</v>
       </c>
       <c r="D3" s="23">
         <f t="shared" si="2"/>
@@ -2342,11 +2348,11 @@
       </c>
       <c r="B4" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="23">
         <f t="shared" si="2"/>
@@ -2432,7 +2438,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2470,7 +2476,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3917,7 +3923,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C10"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3962,7 +3968,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5515,7 +5521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
@@ -7199,9 +7205,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Cadastro de idiomas Tela e Maps
</commit_message>
<xml_diff>
--- a/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
+++ b/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Graficos" sheetId="7" r:id="rId1"/>
@@ -1699,10 +1699,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -1718,25 +1718,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="131025920"/>
-        <c:axId val="131031808"/>
+        <c:axId val="132402176"/>
+        <c:axId val="132412160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="131025920"/>
+        <c:axId val="132402176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131031808"/>
+        <c:crossAx val="132412160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131031808"/>
+        <c:axId val="132412160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1762,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131025920"/>
+        <c:crossAx val="132402176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1774,7 +1774,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000147" footer="0.31496062000000147"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000152" footer="0.31496062000000152"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1839,10 +1839,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1861,24 +1861,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="131056768"/>
-        <c:axId val="131058304"/>
+        <c:axId val="132428928"/>
+        <c:axId val="132430464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="131056768"/>
+        <c:axId val="132428928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131058304"/>
+        <c:crossAx val="132430464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131058304"/>
+        <c:axId val="132430464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1886,7 +1886,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131056768"/>
+        <c:crossAx val="132428928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1898,7 +1898,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="E2" s="21">
         <f t="shared" ref="E2:E7" si="3">COUNTIF(StatusTasks,A2)</f>
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2339,11 +2339,11 @@
       </c>
       <c r="D3" s="23">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2360,7 +2360,7 @@
       </c>
       <c r="D4" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="24">
         <f t="shared" si="3"/>
@@ -5525,9 +5525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -5608,7 +5608,7 @@
         <v>30</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7209,9 +7209,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7400,7 +7400,7 @@
         <v>43</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7418,7 +7418,7 @@
         <v>44</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -7436,7 +7436,7 @@
         <v>45</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -7454,7 +7454,7 @@
         <v>76</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5">

</xml_diff>

<commit_message>
Tela novo idioma - mensagem
</commit_message>
<xml_diff>
--- a/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
+++ b/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
@@ -1508,7 +1508,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1719,25 +1718,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="111365120"/>
-        <c:axId val="111371008"/>
+        <c:axId val="113662976"/>
+        <c:axId val="113672960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111365120"/>
+        <c:axId val="113662976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111371008"/>
+        <c:crossAx val="113672960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111371008"/>
+        <c:axId val="113672960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1759,25 +1758,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111365120"/>
+        <c:crossAx val="113662976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000158" footer="0.31496062000000158"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000163" footer="0.31496062000000163"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1787,9 +1784,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1847,13 +1842,13 @@
                   <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1866,24 +1861,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="111395968"/>
-        <c:axId val="111397504"/>
+        <c:axId val="113693824"/>
+        <c:axId val="113695360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111395968"/>
+        <c:axId val="113693824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111397504"/>
+        <c:crossAx val="113695360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111397504"/>
+        <c:axId val="113695360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1891,20 +1886,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111395968"/>
+        <c:crossAx val="113693824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000091" footer="0.31496062000000091"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000097" footer="0.31496062000000097"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2349,7 +2343,7 @@
       </c>
       <c r="E3" s="24">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2391,7 +2385,7 @@
       </c>
       <c r="E5" s="24">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7217,7 +7211,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7424,7 +7418,7 @@
         <v>44</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>

<commit_message>
Adicionar idioma, mensagens, testes
</commit_message>
<xml_diff>
--- a/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
+++ b/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="7800" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Graficos" sheetId="7" r:id="rId1"/>
@@ -1842,13 +1842,13 @@
                   <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="E3" s="24">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E5" s="24">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7211,7 +7211,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7436,7 +7436,7 @@
         <v>45</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5">

</xml_diff>

<commit_message>
Tela de Edição de Idioma
</commit_message>
<xml_diff>
--- a/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
+++ b/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
@@ -1718,25 +1718,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="131292160"/>
-        <c:axId val="131302144"/>
+        <c:axId val="106322944"/>
+        <c:axId val="106332928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="131292160"/>
+        <c:axId val="106322944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131302144"/>
+        <c:crossAx val="106332928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131302144"/>
+        <c:axId val="106332928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1762,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131292160"/>
+        <c:crossAx val="106322944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1774,7 +1774,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000175" footer="0.31496062000000175"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000186" footer="0.31496062000000186"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1839,16 +1839,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1861,24 +1861,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="131318912"/>
-        <c:axId val="131320448"/>
+        <c:axId val="106353792"/>
+        <c:axId val="106355328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="131318912"/>
+        <c:axId val="106353792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131320448"/>
+        <c:crossAx val="106355328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131320448"/>
+        <c:axId val="106355328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1886,7 +1886,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131318912"/>
+        <c:crossAx val="106353792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1898,7 +1898,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000102" footer="0.31496062000000102"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000108" footer="0.31496062000000108"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="E2" s="21">
         <f t="shared" ref="E2:E7" si="3">COUNTIF(StatusTasks,A2)</f>
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="E3" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E5" s="24">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7211,7 +7211,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7472,7 +7472,7 @@
         <v>48</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -7490,7 +7490,7 @@
         <v>49</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7508,7 +7508,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -7526,7 +7526,7 @@
         <v>51</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5">

</xml_diff>

<commit_message>
Testes e RF salvar idiomas editados
</commit_message>
<xml_diff>
--- a/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
+++ b/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
@@ -1718,25 +1718,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="106322944"/>
-        <c:axId val="106332928"/>
+        <c:axId val="103767040"/>
+        <c:axId val="103789312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106322944"/>
+        <c:axId val="103767040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106332928"/>
+        <c:crossAx val="103789312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106332928"/>
+        <c:axId val="103789312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1762,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106322944"/>
+        <c:crossAx val="103767040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1774,7 +1774,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000186" footer="0.31496062000000186"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000191" footer="0.31496062000000191"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1839,16 +1839,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1861,24 +1861,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="106353792"/>
-        <c:axId val="106355328"/>
+        <c:axId val="103801984"/>
+        <c:axId val="103803520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106353792"/>
+        <c:axId val="103801984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106355328"/>
+        <c:crossAx val="103803520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106355328"/>
+        <c:axId val="103803520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1886,7 +1886,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106353792"/>
+        <c:crossAx val="103801984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1898,7 +1898,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000108" footer="0.31496062000000108"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000113" footer="0.31496062000000113"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="E2" s="21">
         <f t="shared" ref="E2:E7" si="3">COUNTIF(StatusTasks,A2)</f>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="E3" s="24">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E5" s="24">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7211,7 +7211,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7490,7 +7490,7 @@
         <v>49</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7508,7 +7508,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -7526,7 +7526,7 @@
         <v>51</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5">

</xml_diff>

<commit_message>
Tela/ Contratos / implementação Mostrar Generos
</commit_message>
<xml_diff>
--- a/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
+++ b/_Docs/0 - Agile Managment - Projeto BiblioE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="7800" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="7800" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Graficos" sheetId="7" r:id="rId1"/>
@@ -687,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -779,6 +779,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1699,10 +1702,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -1718,25 +1721,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="135425024"/>
-        <c:axId val="135435008"/>
+        <c:axId val="128871424"/>
+        <c:axId val="128881408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135425024"/>
+        <c:axId val="128871424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135435008"/>
+        <c:crossAx val="128881408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135435008"/>
+        <c:axId val="128881408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1765,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135425024"/>
+        <c:crossAx val="128871424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1774,7 +1777,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000197" footer="0.31496062000000197"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000202" footer="0.31496062000000202"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1839,16 +1842,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1861,24 +1864,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="135451776"/>
-        <c:axId val="135453312"/>
+        <c:axId val="128902272"/>
+        <c:axId val="128903808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135451776"/>
+        <c:axId val="128902272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135453312"/>
+        <c:crossAx val="128903808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135453312"/>
+        <c:axId val="128903808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1886,7 +1889,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135451776"/>
+        <c:crossAx val="128902272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1898,7 +1901,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000125" footer="0.31496062000000125"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000136" footer="0.31496062000000136"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2322,7 +2325,7 @@
       </c>
       <c r="E2" s="21">
         <f t="shared" ref="E2:E7" si="3">COUNTIF(StatusTasks,A2)</f>
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2339,11 +2342,11 @@
       </c>
       <c r="D3" s="23">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2360,11 +2363,11 @@
       </c>
       <c r="D4" s="23">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2385,7 +2388,7 @@
       </c>
       <c r="E5" s="24">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5525,9 +5528,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -5661,8 +5664,8 @@
       <c r="D7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>6</v>
+      <c r="E7" s="42" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -7209,9 +7212,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7544,7 +7547,7 @@
         <v>52</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -7562,7 +7565,7 @@
         <v>53</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -7597,8 +7600,8 @@
       <c r="D21" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="31" t="s">
-        <v>7</v>
+      <c r="E21" s="43" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -7616,7 +7619,7 @@
         <v>62</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -7634,7 +7637,7 @@
         <v>63</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -7652,7 +7655,7 @@
         <v>64</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5">

</xml_diff>